<commit_message>
Add some extra information to style extracted from file
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -25,7 +25,7 @@
     <t>Bar</t>
   </si>
   <si>
-    <t>Baz </t>
+    <t>Baz</t>
   </si>
   <si>
     <t>Quuk</t>
@@ -76,7 +76,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -84,38 +84,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42">
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9">
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -199,7 +229,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -215,11 +245,11 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test copying Font information into user level cell style.
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -232,7 +232,8 @@
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15">
+  </sheetFormatPr>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
   </cols>
@@ -258,8 +259,10 @@
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>
+    </oddHeader>
+    <oddFooter>
+    </oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -275,7 +278,8 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15">
+  </sheetFormatPr>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
   </cols>
@@ -284,8 +288,10 @@
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>
+    </oddHeader>
+    <oddFooter>
+    </oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>